<commit_message>
arrumar logo e finalizar paleta de cores
</commit_message>
<xml_diff>
--- a/Paleta de Cores e Tipografia.xlsx
+++ b/Paleta de Cores e Tipografia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sesisenaispedu-my.sharepoint.com/personal/emilly_nascimento_portalsesisp_org_br/Documents/SENAI - 2025 - DS/LIMA/Atividade - Startup de finanças/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{9DD9200A-66C4-4667-B6CE-92B43C7D81A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E87BE55-4B54-4566-963A-08C6D385D61A}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{9DD9200A-66C4-4667-B6CE-92B43C7D81A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55BA09C0-F31C-425D-82C7-071EA0A41615}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{469993F3-5E49-4EE9-B447-E4441C5BDD9B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>Onde utilizar?</t>
   </si>
@@ -217,7 +217,7 @@
     <t>rgb(153, 248, 191)</t>
   </si>
   <si>
-    <t>h2, h2</t>
+    <t>h2, h3</t>
   </si>
   <si>
     <t>rgb(0, 0, 0)</t>
@@ -268,7 +268,7 @@
     <t>#f8fcf9</t>
   </si>
   <si>
-    <t>h2 dos cards</t>
+    <t>h2 dos cards, texto final</t>
   </si>
   <si>
     <t>Subtítulo dos cards</t>
@@ -280,7 +280,7 @@
     <t>Itens do card</t>
   </si>
   <si>
-    <t>Es</t>
+    <t>h2 do blog</t>
   </si>
 </sst>
 </file>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83D3F93-F33A-4F07-AAFC-F090ED020D6A}">
   <dimension ref="B2:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1044,7 +1044,9 @@
       <c r="B35" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>